<commit_message>
Backlog - Versão final
</commit_message>
<xml_diff>
--- a/Ferramenta de Gestão/Projeto_individual.xlsx
+++ b/Ferramenta de Gestão/Projeto_individual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samar\Downloads\Projeto-Individual---SPTech\Ferramenta de Gestão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F83EFCD-262E-4E15-B988-90FA1B7B328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5761C3B9-74F1-4791-AA70-7192E43E559C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -169,12 +169,6 @@
   </si>
   <si>
     <t>IMPORTANTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colocar check de estrelas </t>
-  </si>
-  <si>
-    <t>Como meio de avaliar os livros, com base nas suas leituras</t>
   </si>
   <si>
     <t>DESEJÁVEL</t>
@@ -560,7 +554,7 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>29</c:v>
@@ -636,7 +630,7 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>29</c:v>
@@ -1380,15 +1374,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1581150</xdr:colOff>
+      <xdr:colOff>1757711</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:rowOff>142412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4505325</xdr:colOff>
+      <xdr:colOff>4681886</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1059562</xdr:rowOff>
+      <xdr:rowOff>1078148</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1417,7 +1411,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3629025" y="123826"/>
+          <a:off x="3969370" y="142412"/>
           <a:ext cx="2924175" cy="935736"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1437,7 +1431,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>111512</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>1858</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1785,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1839,7 +1833,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>6</v>
@@ -1881,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>16</v>
@@ -1893,8 +1887,8 @@
         <v>17</v>
       </c>
       <c r="L3" s="5">
-        <f>SUM(E3:E19)</f>
-        <v>134</v>
+        <f>SUM(E3:E18)</f>
+        <v>126</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1920,7 +1914,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>16</v>
@@ -1929,22 +1923,22 @@
         <v>10</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L4" s="5">
-        <f>SUMIF($G$3:$G$19,K4,$E$3:$E$19)</f>
+        <f>SUMIF($G$3:$G$18,K4,$E$3:$E$18)</f>
         <v>21</v>
       </c>
       <c r="M4" s="5">
-        <f>SUMIF($G$3:$G$19,K4,$E$3:$E$19)</f>
+        <f>SUMIF($G$3:$G$18,K4,$E$3:$E$18)</f>
         <v>21</v>
       </c>
       <c r="N4" s="5">
-        <f>SUMIFS($E$3:$E$19,$I$3:$I$19,$N$2,$G$3:$G$19,K4)</f>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$N$2,$G$3:$G$18,K4)</f>
         <v>21</v>
       </c>
       <c r="O4" s="5">
-        <f>SUMIFS($E$3:$E$19,$I$3:$I$19,$O$2,$G$3:$G$19,K4)</f>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$O$2,$G$3:$G$18,K4)</f>
         <v>0</v>
       </c>
     </row>
@@ -1968,7 +1962,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>16</v>
@@ -1977,22 +1971,22 @@
         <v>10</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L5" s="5">
-        <f t="shared" ref="L5:L7" si="0">SUMIF($G$3:$G$19,K5,$E$3:$E$19)</f>
+        <f>SUMIF($G$3:$G$18,K5,$E$3:$E$18)</f>
         <v>34</v>
       </c>
       <c r="M5" s="5">
-        <f t="shared" ref="M5:M7" si="1">SUMIF($G$3:$G$19,K5,$E$3:$E$19)</f>
+        <f>SUMIF($G$3:$G$18,K5,$E$3:$E$18)</f>
         <v>34</v>
       </c>
       <c r="N5" s="5">
-        <f t="shared" ref="N5:N7" si="2">SUMIFS($E$3:$E$19,$I$3:$I$19,$N$2,$G$3:$G$19,K5)</f>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$N$2,$G$3:$G$18,K5)</f>
         <v>34</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" ref="O5:O7" si="3">SUMIFS($E$3:$E$19,$I$3:$I$19,$O$2,$G$3:$G$19,K5)</f>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$O$2,$G$3:$G$18,K5)</f>
         <v>0</v>
       </c>
     </row>
@@ -2016,7 +2010,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>16</v>
@@ -2025,22 +2019,22 @@
         <v>10</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L6" s="5">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <f>SUMIF($G$3:$G$18,K6,$E$3:$E$18)</f>
+        <v>42</v>
       </c>
       <c r="M6" s="5">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f>SUMIF($G$3:$G$18,K6,$E$3:$E$18)</f>
+        <v>42</v>
       </c>
       <c r="N6" s="5">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$N$2,$G$3:$G$18,K6)</f>
+        <v>42</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="3"/>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$O$2,$G$3:$G$18,K6)</f>
         <v>0</v>
       </c>
     </row>
@@ -2064,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>16</v>
@@ -2073,22 +2067,22 @@
         <v>10</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L7" s="5">
-        <f t="shared" si="0"/>
+        <f>SUMIF($G$3:$G$18,K7,$E$3:$E$18)</f>
         <v>29</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" si="1"/>
+        <f>SUMIF($G$3:$G$18,K7,$E$3:$E$18)</f>
         <v>29</v>
       </c>
       <c r="N7" s="5">
-        <f t="shared" si="2"/>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$N$2,$G$3:$G$18,K7)</f>
         <v>29</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="3"/>
+        <f>SUMIFS($E$3:$E$18,$I$3:$I$18,$O$2,$G$3:$G$18,K7)</f>
         <v>0</v>
       </c>
     </row>
@@ -2112,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>16</v>
@@ -2141,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>16</v>
@@ -2170,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>16</v>
@@ -2199,7 +2193,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>16</v>
@@ -2228,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>16</v>
@@ -2257,7 +2251,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>16</v>
@@ -2286,7 +2280,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>16</v>
@@ -2297,13 +2291,13 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>25</v>
@@ -2315,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>16</v>
@@ -2344,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>16</v>
@@ -2373,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>16</v>
@@ -2393,50 +2387,21 @@
         <v>14</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E18" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F18" s="5">
         <v>1</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="5">
-        <v>13</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2455,7 +2420,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C3:C19</xm:sqref>
+          <xm:sqref>C3:C18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -2464,7 +2429,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D3:D19</xm:sqref>
+          <xm:sqref>D3:D18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -2473,7 +2438,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>E3:E19</xm:sqref>
+          <xm:sqref>E3:E18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -2482,7 +2447,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>I3:I19</xm:sqref>
+          <xm:sqref>I3:I18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2511,7 +2476,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>7</v>
@@ -2545,7 +2510,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2571,7 +2536,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="9">
         <v>21</v>
@@ -2591,7 +2556,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="9">
         <f>Backlog!M4</f>
@@ -2604,7 +2569,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="9">
         <f>Backlog!M5</f>
@@ -2617,20 +2582,20 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="9">
         <f>Backlog!M6</f>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C15" s="9">
         <f>Backlog!N6</f>
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="9">
         <f>Backlog!M7</f>

</xml_diff>